<commit_message>
Adding Ext3 in IO definition excel sheet.
</commit_message>
<xml_diff>
--- a/Designs/IO Definitions for SAMD21 Xplained Pro Dev Kit.xlsx
+++ b/Designs/IO Definitions for SAMD21 Xplained Pro Dev Kit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
   <si>
     <t xml:space="preserve">Header</t>
   </si>
@@ -134,6 +134,45 @@
   </si>
   <si>
     <t xml:space="preserve">PA19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ext3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB23</t>
   </si>
 </sst>
 </file>
@@ -148,6 +187,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -170,6 +210,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,11 +260,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -240,16 +281,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -489,25 +530,19 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,10 +550,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,10 +561,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,10 +572,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,10 +583,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,10 +594,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,10 +605,10 @@
         <v>23</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,10 +616,10 @@
         <v>23</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,10 +627,10 @@
         <v>23</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,10 +638,10 @@
         <v>23</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,10 +649,10 @@
         <v>23</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,10 +660,10 @@
         <v>23</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,10 +671,10 @@
         <v>23</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,10 +682,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,10 +693,10 @@
         <v>23</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,10 +704,10 @@
         <v>23</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,10 +715,10 @@
         <v>23</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -691,10 +726,10 @@
         <v>23</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,9 +737,240 @@
         <v>23</v>
       </c>
       <c r="B41" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>